<commit_message>
add info to final project rubric
</commit_message>
<xml_diff>
--- a/management/Final Project Rubric.xlsx
+++ b/management/Final Project Rubric.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CSC4992Project\management\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BE68B44-F364-47D3-B198-61DED43F996C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C1082BB-A9BB-4619-B7EE-EFDA58BCD0F3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12060" windowHeight="4860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12060" windowHeight="4860" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Group rubrik" sheetId="3" r:id="rId1"/>
-    <sheet name="Individual rubrik" sheetId="4" r:id="rId2"/>
+    <sheet name="Individual rubrik (4)" sheetId="7" r:id="rId2"/>
+    <sheet name="Individual rubrik (3)" sheetId="6" r:id="rId3"/>
+    <sheet name="Individual rubrik (2)" sheetId="5" r:id="rId4"/>
+    <sheet name="Individual rubrik" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -31,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="525" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="67">
   <si>
     <t>Earned</t>
   </si>
@@ -226,6 +229,12 @@
   </si>
   <si>
     <t>For loop, CardDeck.py: set up rows of cards; If statements, CardDeck.py: check if cards match</t>
+  </si>
+  <si>
+    <t>Student: Kevin Zhang</t>
+  </si>
+  <si>
+    <t>Set up pygame infrastructure (game loops, game display). Coded main single player gameplay. Saved and read scores from multiple different csv files based on different settings.</t>
   </si>
 </sst>
 </file>
@@ -428,13 +437,13 @@
     <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
@@ -753,7 +762,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C40D522-ECA1-FF4D-B661-39278A20B6C5}">
   <dimension ref="A1:J29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+    <sheetView topLeftCell="A17" workbookViewId="0">
       <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
@@ -769,16 +778,16 @@
   <sheetData>
     <row r="1" spans="1:9" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A1" s="1"/>
-      <c r="B1" s="29" t="s">
+      <c r="B1" s="30" t="s">
         <v>50</v>
       </c>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="F1" s="29" t="s">
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="F1" s="30" t="s">
         <v>51</v>
       </c>
-      <c r="G1" s="29"/>
-      <c r="H1" s="29"/>
+      <c r="G1" s="30"/>
+      <c r="H1" s="30"/>
     </row>
     <row r="2" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A2" s="1"/>
@@ -1079,7 +1088,7 @@
       <c r="I19" s="18" t="s">
         <v>64</v>
       </c>
-      <c r="J19" s="31"/>
+      <c r="J19" s="29"/>
     </row>
     <row r="20" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="12" t="s">
@@ -1326,6 +1335,480 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F0755B4-2AC8-4691-A690-8656405603A6}">
+  <dimension ref="A1:I12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="3" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="38.28515625" style="2" customWidth="1"/>
+    <col min="3" max="4" width="10.85546875" style="2"/>
+    <col min="5" max="5" width="69.28515625" style="2" customWidth="1"/>
+    <col min="6" max="9" width="32.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="10.85546875" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A1" s="1"/>
+      <c r="B1" s="31" t="s">
+        <v>65</v>
+      </c>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+    </row>
+    <row r="2" spans="1:9" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B2" s="3"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
+    </row>
+    <row r="3" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="C3" s="6"/>
+      <c r="D3" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="E3" s="15"/>
+    </row>
+    <row r="4" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="C4" s="6"/>
+      <c r="D4" s="7">
+        <v>0.1</v>
+      </c>
+      <c r="E4" s="15"/>
+    </row>
+    <row r="5" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A5" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="C5" s="6"/>
+      <c r="D5" s="7">
+        <v>0.2</v>
+      </c>
+      <c r="E5" s="9" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="6"/>
+      <c r="D6" s="7">
+        <v>0.1</v>
+      </c>
+      <c r="E6" s="15"/>
+    </row>
+    <row r="7" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="C7" s="6"/>
+      <c r="D7" s="7">
+        <v>0.1</v>
+      </c>
+      <c r="E7" s="15"/>
+    </row>
+    <row r="8" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B8" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" s="14">
+        <f>SUM(C3:C7)</f>
+        <v>0</v>
+      </c>
+      <c r="D8" s="14">
+        <f>SUM(D3:D7)</f>
+        <v>1</v>
+      </c>
+      <c r="E8" s="15"/>
+      <c r="F8" s="15"/>
+      <c r="G8" s="15"/>
+      <c r="H8" s="15"/>
+      <c r="I8" s="15"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E9" s="15"/>
+      <c r="F9" s="15"/>
+      <c r="G9" s="15"/>
+      <c r="H9" s="15"/>
+      <c r="I9" s="15"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E10" s="15"/>
+      <c r="F10" s="15"/>
+      <c r="G10" s="15"/>
+      <c r="H10" s="15"/>
+      <c r="I10" s="15"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E11" s="15"/>
+      <c r="F11" s="15"/>
+      <c r="G11" s="15"/>
+      <c r="H11" s="15"/>
+      <c r="I11" s="15"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E12" s="15"/>
+      <c r="F12" s="15"/>
+      <c r="G12" s="15"/>
+      <c r="H12" s="15"/>
+      <c r="I12" s="15"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B1:E1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C40E83DE-F0AE-4BE2-8626-A90FC296FE5D}">
+  <dimension ref="A1:I12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="3" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="38.28515625" style="2" customWidth="1"/>
+    <col min="3" max="4" width="10.85546875" style="2"/>
+    <col min="5" max="5" width="69.28515625" style="2" customWidth="1"/>
+    <col min="6" max="9" width="32.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="10.85546875" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A1" s="1"/>
+      <c r="B1" s="31" t="s">
+        <v>41</v>
+      </c>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+    </row>
+    <row r="2" spans="1:9" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B2" s="3"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
+    </row>
+    <row r="3" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="C3" s="6"/>
+      <c r="D3" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="E3" s="15"/>
+    </row>
+    <row r="4" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="C4" s="6"/>
+      <c r="D4" s="7">
+        <v>0.1</v>
+      </c>
+      <c r="E4" s="15"/>
+    </row>
+    <row r="5" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="C5" s="6"/>
+      <c r="D5" s="7">
+        <v>0.2</v>
+      </c>
+      <c r="E5" s="9" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="6"/>
+      <c r="D6" s="7">
+        <v>0.1</v>
+      </c>
+      <c r="E6" s="15"/>
+    </row>
+    <row r="7" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="C7" s="6"/>
+      <c r="D7" s="7">
+        <v>0.1</v>
+      </c>
+      <c r="E7" s="15"/>
+    </row>
+    <row r="8" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B8" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" s="14">
+        <f>SUM(C3:C7)</f>
+        <v>0</v>
+      </c>
+      <c r="D8" s="14">
+        <f>SUM(D3:D7)</f>
+        <v>1</v>
+      </c>
+      <c r="E8" s="15"/>
+      <c r="F8" s="15"/>
+      <c r="G8" s="15"/>
+      <c r="H8" s="15"/>
+      <c r="I8" s="15"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E9" s="15"/>
+      <c r="F9" s="15"/>
+      <c r="G9" s="15"/>
+      <c r="H9" s="15"/>
+      <c r="I9" s="15"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E10" s="15"/>
+      <c r="F10" s="15"/>
+      <c r="G10" s="15"/>
+      <c r="H10" s="15"/>
+      <c r="I10" s="15"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E11" s="15"/>
+      <c r="F11" s="15"/>
+      <c r="G11" s="15"/>
+      <c r="H11" s="15"/>
+      <c r="I11" s="15"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E12" s="15"/>
+      <c r="F12" s="15"/>
+      <c r="G12" s="15"/>
+      <c r="H12" s="15"/>
+      <c r="I12" s="15"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B1:E1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE538CBB-882A-46F4-97EB-96C43E708189}">
+  <dimension ref="A1:I12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="3" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="38.28515625" style="2" customWidth="1"/>
+    <col min="3" max="4" width="10.85546875" style="2"/>
+    <col min="5" max="5" width="69.28515625" style="2" customWidth="1"/>
+    <col min="6" max="9" width="32.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="10.85546875" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A1" s="1"/>
+      <c r="B1" s="31" t="s">
+        <v>41</v>
+      </c>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+    </row>
+    <row r="2" spans="1:9" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B2" s="3"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
+    </row>
+    <row r="3" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="C3" s="6"/>
+      <c r="D3" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="E3" s="15"/>
+    </row>
+    <row r="4" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="C4" s="6"/>
+      <c r="D4" s="7">
+        <v>0.1</v>
+      </c>
+      <c r="E4" s="15"/>
+    </row>
+    <row r="5" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="C5" s="6"/>
+      <c r="D5" s="7">
+        <v>0.2</v>
+      </c>
+      <c r="E5" s="9" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="6"/>
+      <c r="D6" s="7">
+        <v>0.1</v>
+      </c>
+      <c r="E6" s="15"/>
+    </row>
+    <row r="7" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="C7" s="6"/>
+      <c r="D7" s="7">
+        <v>0.1</v>
+      </c>
+      <c r="E7" s="15"/>
+    </row>
+    <row r="8" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B8" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" s="14">
+        <f>SUM(C3:C7)</f>
+        <v>0</v>
+      </c>
+      <c r="D8" s="14">
+        <f>SUM(D3:D7)</f>
+        <v>1</v>
+      </c>
+      <c r="E8" s="15"/>
+      <c r="F8" s="15"/>
+      <c r="G8" s="15"/>
+      <c r="H8" s="15"/>
+      <c r="I8" s="15"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E9" s="15"/>
+      <c r="F9" s="15"/>
+      <c r="G9" s="15"/>
+      <c r="H9" s="15"/>
+      <c r="I9" s="15"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E10" s="15"/>
+      <c r="F10" s="15"/>
+      <c r="G10" s="15"/>
+      <c r="H10" s="15"/>
+      <c r="I10" s="15"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E11" s="15"/>
+      <c r="F11" s="15"/>
+      <c r="G11" s="15"/>
+      <c r="H11" s="15"/>
+      <c r="I11" s="15"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E12" s="15"/>
+      <c r="F12" s="15"/>
+      <c r="G12" s="15"/>
+      <c r="H12" s="15"/>
+      <c r="I12" s="15"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B1:E1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A78C414E-0631-754C-9D21-42920DF019FE}">
   <dimension ref="A1:I12"/>
   <sheetViews>
@@ -1345,12 +1828,12 @@
   <sheetData>
     <row r="1" spans="1:9" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A1" s="1"/>
-      <c r="B1" s="30" t="s">
+      <c r="B1" s="31" t="s">
         <v>41</v>
       </c>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
     </row>
     <row r="2" spans="1:9" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B2" s="3"/>

</xml_diff>